<commit_message>
membuat fitur menambahkan simpanan dengan banuak member
</commit_message>
<xml_diff>
--- a/database/data/demoSaving.xlsx
+++ b/database/data/demoSaving.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projek Sekolah\koperasi-api\database\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIN WEB\GIN WEB\project\Koperasi App\koperasi-api\database\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3E6A684-8C36-4C93-9590-013F56970824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886534AE-25F6-4D21-8D43-98A0A46804EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD6C993E-35EF-45D6-B763-96DCA252CEDA}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{DD6C993E-35EF-45D6-B763-96DCA252CEDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>NO</t>
   </si>
@@ -154,6 +145,12 @@
   </si>
   <si>
     <t>Ismi</t>
+  </si>
+  <si>
+    <t>bulan pembayaran</t>
+  </si>
+  <si>
+    <t>juli 2023</t>
   </si>
 </sst>
 </file>
@@ -163,7 +160,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +234,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Abadi MT Condensed Light"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Abadi MT Condensed Light"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -252,7 +260,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -409,13 +417,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -448,7 +493,6 @@
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -458,7 +502,6 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -471,6 +514,14 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -787,27 +838,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9151EA3F-1A5D-408E-8B35-68089BA02C75}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="41.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="32" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="48.6" thickTop="1">
+    <row r="1" spans="1:13" ht="24.75" thickTop="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -841,11 +893,14 @@
       <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" s="8">
         <v>5</v>
       </c>
@@ -872,12 +927,15 @@
       <c r="J2" s="11">
         <v>40000</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="12">
+      <c r="K2" s="31"/>
+      <c r="L2" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="12">
         <v>1005000</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="8">
         <v>6</v>
       </c>
@@ -900,12 +958,15 @@
       <c r="J3" s="11">
         <v>20000</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="12">
+      <c r="K3" s="31"/>
+      <c r="L3" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="12">
         <v>150000</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="20.399999999999999">
+    <row r="4" spans="1:13">
       <c r="A4" s="8">
         <v>7</v>
       </c>
@@ -934,14 +995,17 @@
       <c r="J4" s="15">
         <v>20000</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="32">
         <v>100000</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="12">
         <v>710000</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30.6">
+    <row r="5" spans="1:13">
       <c r="A5" s="8">
         <v>8</v>
       </c>
@@ -968,14 +1032,17 @@
       <c r="J5" s="15">
         <v>20000</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="31">
         <v>250000</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="12">
         <v>500000</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30.6">
+    <row r="6" spans="1:13">
       <c r="A6" s="8">
         <v>9</v>
       </c>
@@ -998,19 +1065,22 @@
       <c r="J6" s="15">
         <v>20000</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="12">
+      <c r="K6" s="31"/>
+      <c r="L6" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" s="12">
         <v>75000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30.6">
+    <row r="7" spans="1:13">
       <c r="A7" s="8">
         <v>10</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="16">
         <v>110000</v>
       </c>
       <c r="D7" s="14">
@@ -1028,14 +1098,17 @@
       <c r="J7" s="15">
         <v>20000</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="33">
         <v>460000</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="12">
         <v>645000</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="51">
+    <row r="8" spans="1:13">
       <c r="A8" s="8">
         <v>11</v>
       </c>
@@ -1060,12 +1133,15 @@
       <c r="J8" s="15">
         <v>20000</v>
       </c>
-      <c r="K8" s="10"/>
-      <c r="L8" s="12">
+      <c r="K8" s="31"/>
+      <c r="L8" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" s="12">
         <v>265000</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30.6">
+    <row r="9" spans="1:13">
       <c r="A9" s="8">
         <v>12</v>
       </c>
@@ -1090,19 +1166,22 @@
       <c r="J9" s="15">
         <v>20000</v>
       </c>
-      <c r="K9" s="10"/>
-      <c r="L9" s="12">
+      <c r="K9" s="31"/>
+      <c r="L9" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" s="12">
         <v>350000</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30.6">
+    <row r="10" spans="1:13">
       <c r="A10" s="8">
         <v>13</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="16">
         <v>110000</v>
       </c>
       <c r="D10" s="14">
@@ -1120,12 +1199,15 @@
       <c r="J10" s="15">
         <v>20000</v>
       </c>
-      <c r="K10" s="10"/>
-      <c r="L10" s="12">
+      <c r="K10" s="31"/>
+      <c r="L10" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" s="12">
         <v>210000</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30.6">
+    <row r="11" spans="1:13">
       <c r="A11" s="8">
         <v>14</v>
       </c>
@@ -1150,19 +1232,22 @@
       <c r="J11" s="15">
         <v>20000</v>
       </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="12">
+      <c r="K11" s="31"/>
+      <c r="L11" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" s="12">
         <v>3150000</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12" s="8">
         <v>15</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="14">
         <v>25000</v>
       </c>
@@ -1178,16 +1263,19 @@
       <c r="J12" s="15">
         <v>20000</v>
       </c>
-      <c r="K12" s="10"/>
-      <c r="L12" s="12">
+      <c r="K12" s="31"/>
+      <c r="L12" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M12" s="12">
         <v>100000</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" s="8">
         <v>16</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="10"/>
@@ -1206,16 +1294,19 @@
       <c r="J13" s="15">
         <v>20000</v>
       </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="12">
+      <c r="K13" s="31"/>
+      <c r="L13" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M13" s="12">
         <v>100000</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" s="8">
         <v>17</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="10"/>
@@ -1235,22 +1326,25 @@
         <v>150000</v>
       </c>
       <c r="I14" s="12"/>
-      <c r="J14" s="20">
-        <v>20000</v>
-      </c>
-      <c r="K14" s="10"/>
-      <c r="L14" s="12">
+      <c r="J14" s="19">
+        <v>20000</v>
+      </c>
+      <c r="K14" s="31"/>
+      <c r="L14" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M14" s="12">
         <v>1250000</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="A15" s="8">
         <v>18</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="14">
         <v>25000</v>
       </c>
@@ -1270,12 +1364,15 @@
       <c r="J15" s="15">
         <v>20000</v>
       </c>
-      <c r="K15" s="22"/>
-      <c r="L15" s="12">
+      <c r="K15" s="34"/>
+      <c r="L15" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M15" s="12">
         <v>725000</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16" s="8">
         <v>20</v>
       </c>
@@ -1300,12 +1397,15 @@
       <c r="J16" s="15">
         <v>20000</v>
       </c>
-      <c r="K16" s="10"/>
-      <c r="L16" s="12">
+      <c r="K16" s="31"/>
+      <c r="L16" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M16" s="12">
         <v>200000</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:13">
       <c r="A17" s="8">
         <v>21</v>
       </c>
@@ -1328,19 +1428,22 @@
       <c r="J17" s="15">
         <v>20000</v>
       </c>
-      <c r="K17" s="10"/>
-      <c r="L17" s="12">
+      <c r="K17" s="31"/>
+      <c r="L17" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M17" s="12">
         <v>100000</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:13">
       <c r="A18" s="8">
         <v>22</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="23">
+      <c r="C18" s="21">
         <v>110000</v>
       </c>
       <c r="D18" s="14">
@@ -1358,13 +1461,16 @@
       <c r="J18" s="15">
         <v>20000</v>
       </c>
-      <c r="K18" s="10"/>
-      <c r="L18" s="12">
+      <c r="K18" s="31"/>
+      <c r="L18" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M18" s="12">
         <v>360000</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="24">
+    <row r="19" spans="1:13">
+      <c r="A19" s="22">
         <v>20</v>
       </c>
       <c r="B19" s="9" t="s">
@@ -1388,13 +1494,16 @@
       <c r="J19" s="11">
         <v>20000</v>
       </c>
-      <c r="K19" s="10"/>
-      <c r="L19" s="12">
+      <c r="K19" s="31"/>
+      <c r="L19" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M19" s="12">
         <v>100000</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="24">
+    <row r="20" spans="1:13">
+      <c r="A20" s="22">
         <v>21</v>
       </c>
       <c r="B20" s="9" t="s">
@@ -1408,13 +1517,16 @@
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="12">
+      <c r="K20" s="31"/>
+      <c r="L20" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M20" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="24">
+    <row r="21" spans="1:13">
+      <c r="A21" s="22">
         <v>22</v>
       </c>
       <c r="B21" s="9" t="s">
@@ -1442,13 +1554,16 @@
       <c r="J21" s="11">
         <v>20000</v>
       </c>
-      <c r="K21" s="10"/>
-      <c r="L21" s="12">
+      <c r="K21" s="31"/>
+      <c r="L21" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M21" s="12">
         <v>2007000</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="24">
+    <row r="22" spans="1:13">
+      <c r="A22" s="22">
         <v>23</v>
       </c>
       <c r="B22" s="9" t="s">
@@ -1472,13 +1587,16 @@
       <c r="J22" s="11">
         <v>20000</v>
       </c>
-      <c r="K22" s="10"/>
-      <c r="L22" s="12">
+      <c r="K22" s="31"/>
+      <c r="L22" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M22" s="12">
         <v>225000</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="24">
+    <row r="23" spans="1:13">
+      <c r="A23" s="22">
         <v>24</v>
       </c>
       <c r="B23" s="9" t="s">
@@ -1502,13 +1620,16 @@
       <c r="J23" s="11">
         <v>20000</v>
       </c>
-      <c r="K23" s="10"/>
-      <c r="L23" s="12">
+      <c r="K23" s="31"/>
+      <c r="L23" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M23" s="12">
         <v>125000</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1">
-      <c r="A24" s="24">
+    <row r="24" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A24" s="22">
         <v>25</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -1532,83 +1653,92 @@
       <c r="J24" s="11">
         <v>20000</v>
       </c>
-      <c r="K24" s="10"/>
-      <c r="L24" s="12">
+      <c r="K24" s="31"/>
+      <c r="L24" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M24" s="12">
         <v>125000</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15" thickTop="1">
-      <c r="A25" s="24">
+    <row r="25" spans="1:13" ht="15.75" thickTop="1">
+      <c r="A25" s="22">
         <v>26</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="10"/>
-      <c r="D25" s="25">
-        <v>25000</v>
-      </c>
-      <c r="E25" s="25">
-        <v>5000</v>
-      </c>
-      <c r="F25" s="25">
+      <c r="D25" s="23">
+        <v>25000</v>
+      </c>
+      <c r="E25" s="23">
+        <v>5000</v>
+      </c>
+      <c r="F25" s="23">
         <v>100000</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="23">
         <v>350000</v>
       </c>
-      <c r="H25" s="25">
+      <c r="H25" s="23">
         <v>90000</v>
       </c>
-      <c r="I25" s="25">
+      <c r="I25" s="23">
         <v>0</v>
       </c>
-      <c r="J25" s="26">
-        <v>20000</v>
-      </c>
-      <c r="K25" s="26"/>
-      <c r="L25" s="12">
+      <c r="J25" s="24">
+        <v>20000</v>
+      </c>
+      <c r="K25" s="35"/>
+      <c r="L25" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M25" s="12">
         <v>590000</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="24">
+    <row r="26" spans="1:13">
+      <c r="A26" s="22">
         <v>27</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="27">
+      <c r="C26" s="25">
         <v>220000</v>
       </c>
-      <c r="D26" s="28">
-        <v>25000</v>
-      </c>
-      <c r="E26" s="28">
-        <v>5000</v>
-      </c>
-      <c r="F26" s="28">
+      <c r="D26" s="26">
+        <v>25000</v>
+      </c>
+      <c r="E26" s="26">
+        <v>5000</v>
+      </c>
+      <c r="F26" s="26">
         <v>50000</v>
       </c>
-      <c r="G26" s="28">
+      <c r="G26" s="26">
         <v>250000</v>
       </c>
-      <c r="H26" s="28">
+      <c r="H26" s="26">
         <v>75000</v>
       </c>
-      <c r="I26" s="28"/>
-      <c r="J26" s="29">
-        <v>20000</v>
-      </c>
-      <c r="K26" s="29">
+      <c r="I26" s="26"/>
+      <c r="J26" s="27">
+        <v>20000</v>
+      </c>
+      <c r="K26" s="36">
         <v>260000</v>
       </c>
-      <c r="L26" s="12">
+      <c r="L26" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M26" s="12">
         <v>905000</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="24">
+    <row r="27" spans="1:13">
+      <c r="A27" s="22">
         <v>28</v>
       </c>
       <c r="B27" s="9" t="s">
@@ -1617,32 +1747,35 @@
       <c r="C27" s="10">
         <v>100000</v>
       </c>
-      <c r="D27" s="28">
-        <v>25000</v>
-      </c>
-      <c r="E27" s="28">
-        <v>5000</v>
-      </c>
-      <c r="F27" s="28">
+      <c r="D27" s="26">
+        <v>25000</v>
+      </c>
+      <c r="E27" s="26">
+        <v>5000</v>
+      </c>
+      <c r="F27" s="26">
         <v>50000</v>
       </c>
-      <c r="G27" s="28">
+      <c r="G27" s="26">
         <v>500000</v>
       </c>
-      <c r="H27" s="28">
+      <c r="H27" s="26">
         <v>150000</v>
       </c>
-      <c r="I27" s="28"/>
-      <c r="J27" s="29">
-        <v>20000</v>
-      </c>
-      <c r="K27" s="29"/>
-      <c r="L27" s="12">
+      <c r="I27" s="26"/>
+      <c r="J27" s="27">
+        <v>20000</v>
+      </c>
+      <c r="K27" s="36"/>
+      <c r="L27" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M27" s="12">
         <v>850000</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="24">
+    <row r="28" spans="1:13">
+      <c r="A28" s="22">
         <v>29</v>
       </c>
       <c r="B28" s="9" t="s">
@@ -1664,19 +1797,22 @@
       <c r="J28" s="15">
         <v>20000</v>
       </c>
-      <c r="K28" s="15"/>
-      <c r="L28" s="12">
+      <c r="K28" s="33"/>
+      <c r="L28" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M28" s="12">
         <v>250000</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="30">
+    <row r="29" spans="1:13">
+      <c r="A29" s="28">
         <v>30</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="23"/>
+      <c r="C29" s="21"/>
       <c r="D29" s="14">
         <v>25000</v>
       </c>
@@ -1696,12 +1832,16 @@
       <c r="J29" s="15">
         <v>20000</v>
       </c>
-      <c r="K29" s="15"/>
-      <c r="L29" s="32">
+      <c r="K29" s="33"/>
+      <c r="L29" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="M29" s="30">
         <v>1300000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>